<commit_message>
Improved csv read in
Changed from skiprows to comment in read_csv so variable number of instructions can be included
</commit_message>
<xml_diff>
--- a/author-affiliation-example.xlsx
+++ b/author-affiliation-example.xlsx
@@ -12,21 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
-    <t>Enter names/affiliations as they should be written in LaTeX, e.g. Ren\'{e} for René</t>
+    <t># Enter names/affiliations as they should be written in LaTeX, e.g. Ren\'{e} for René</t>
   </si>
   <si>
-    <t>Additional affiliation columns can be added</t>
+    <t># Additional affiliation columns can be added</t>
   </si>
   <si>
-    <t>Order for first n authors can be set and changed whenever, the list does NOT need to be sorted.</t>
+    <t># Order for first n authors can be set and changed whenever, the list does NOT need to be sorted.</t>
   </si>
   <si>
-    <t>Any author with Order left blank will be sorted automatically in the alphabetical section of the author list</t>
+    <t># Any author with Order left blank will be sorted automatically in the alphabetical section of the author list</t>
   </si>
   <si>
-    <t>Check out: https://github.com/astro-sobrien/latex-author-affiliation-generator</t>
+    <t># Check out: https://github.com/astro-sobrien/latex-author-affiliation-generator</t>
+  </si>
+  <si>
+    <t># Include the hash (#) symbol at the start of any rows containing instructions to co-authors</t>
   </si>
   <si>
     <t>Order</t>
@@ -173,13 +176,13 @@
     <t>Terri</t>
   </si>
   <si>
-    <t>Change the ranges searched in cell B4 so that the entire affiliation range is searched. Currently D5:F9</t>
+    <t># Change the ranges searched in cell B4 so that the entire affiliation range is searched. Currently D5:F9</t>
   </si>
   <si>
-    <t>Ensure that none of the affiliations appear twice due to typos. Any typos must be fixed in the other sheet</t>
+    <t># Ensure that none of the affiliations appear twice due to typos. Any typos must be fixed in the other sheet</t>
   </si>
   <si>
-    <t>Set the commands below. Three-letter codes are not mandatory, avoid using already defined LaTeX commands</t>
+    <t># Set the commands below. Three-letter codes are not mandatory, avoid using already defined LaTeX commands</t>
   </si>
   <si>
     <t>Command</t>
@@ -579,161 +582,158 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="5"/>
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>25</v>
+        <v>3.0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>5.0</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13">
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -743,141 +743,148 @@
         <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17">
       <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18">
       <c r="B18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19">
       <c r="B19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20">
       <c r="B20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21">
       <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22">
       <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23">
-      <c r="C23" s="5"/>
+      <c r="B23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
@@ -8728,6 +8735,14 @@
       <c r="F1004" s="5"/>
       <c r="G1004" s="5"/>
       <c r="H1004" s="5"/>
+    </row>
+    <row r="1005">
+      <c r="C1005" s="5"/>
+      <c r="D1005" s="5"/>
+      <c r="E1005" s="5"/>
+      <c r="F1005" s="5"/>
+      <c r="G1005" s="5"/>
+      <c r="H1005" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -8746,42 +8761,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B5" s="7" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("UNIQUE(FILTER(FLATTEN(Authors_Affiliations!F7:H22),FLATTEN(Authors_Affiliations!F7:H22)&lt;&gt;""""))"),"Department of Affiliation Scripts, University of LaTeX, AB12 3CD, UK")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("UNIQUE(FILTER(FLATTEN(Authors_Affiliations!F8:H23),FLATTEN(Authors_Affiliations!F8:H23)&lt;&gt;""""))"),"Department of Affiliation Scripts, University of LaTeX, AB12 3CD, UK")</f>
         <v>Department of Affiliation Scripts, University of LaTeX, AB12 3CD, UK</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B6" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Centre for Author Lists, University of LaTeX, AB12 3CD, UK")</f>
@@ -8790,7 +8805,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" s="7" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Greendale Community College, Greendale, CO, USA")</f>
@@ -8799,7 +8814,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Indiana University, Bloomington, IN, USA")</f>
@@ -8808,7 +8823,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B9" s="7" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"{\""U}mlaut University, City, Country")</f>
@@ -8817,7 +8832,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B10" s="7" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"City College, Greendale, CO, USA")</f>
@@ -8826,7 +8841,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" s="7" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Greendale Air Conditioning Repair School, Greendale Community College, Greendale, CO, USA")</f>
@@ -8835,7 +8850,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B12" s="7" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Springfield Elementary School, Springfield, State, USA")</f>

</xml_diff>